<commit_message>
latest version of data mapping documents.
Former-commit-id: 0f8240eb0aae09cc06e5a1abc3f4fea0463f3936 [formerly 0f8240eb0aae09cc06e5a1abc3f4fea0463f3936 [formerly 0f8240eb0aae09cc06e5a1abc3f4fea0463f3936 [formerly e332b1fb749fda038665424c83faf6d597791e3a]]]
Former-commit-id: 79a9ac7948a4568b5013b4b0eb35e1cc2571d505
Former-commit-id: 4ee0424e9d304c95b1fb23de7afba0ab9d17fbe9
Former-commit-id: 623328df7db09eaf14141d3d5105f263f6bd4f4c
</commit_message>
<xml_diff>
--- a/data/Data_Mapping _Contracts.xlsx
+++ b/data/Data_Mapping _Contracts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17657" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17657" uniqueCount="231">
   <si>
     <t>UI_element</t>
   </si>
@@ -777,6 +777,12 @@
     <t xml:space="preserve">
 MyMoney Disbursement Open Item Extract v2.10 </t>
   </si>
+  <si>
+    <t>The contract that is active in selected fiscal year. The selected fiscal year should be between Period of Performance start date and end date
+If we have multiple versions consider only the latest version  
+Document Code should be in 
+MA1,MMA1, CT1, CTA1</t>
+  </si>
 </sst>
 </file>
 
@@ -1181,9 +1187,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q1340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1348" sqref="J1348"/>
+      <selection pane="bottomLeft" activeCell="Q386" sqref="Q386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15205,7 +15211,7 @@
         <v>69</v>
       </c>
       <c r="Q332" s="6" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
     </row>
     <row r="333" spans="1:17" x14ac:dyDescent="0.25">
@@ -15572,7 +15578,7 @@
         <v>69</v>
       </c>
       <c r="Q341" s="6" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
     </row>
     <row r="342" spans="1:17" x14ac:dyDescent="0.25">
@@ -16432,7 +16438,7 @@
         <v>69</v>
       </c>
       <c r="Q362" s="6" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
     </row>
     <row r="363" spans="1:17" x14ac:dyDescent="0.25">
@@ -16921,7 +16927,7 @@
         <v>69</v>
       </c>
       <c r="Q374" s="6" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
     </row>
     <row r="375" spans="1:17" x14ac:dyDescent="0.25">
@@ -17410,7 +17416,7 @@
         <v>69</v>
       </c>
       <c r="Q386" s="6" t="s">
-        <v>75</v>
+        <v>230</v>
       </c>
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>